<commit_message>
Working Version 1.0 compiled
</commit_message>
<xml_diff>
--- a/sabr_plan_report/Data/ReportReference.xlsx
+++ b/sabr_plan_report/Data/ReportReference.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="324">
   <si>
     <t>Patient</t>
   </si>
@@ -1182,9 +1182,6 @@
     <t>Chestwall (rib) V50Gy</t>
   </si>
   <si>
-    <t>Proximal Trachea and Bronchial Tree V60Gy</t>
-  </si>
-  <si>
     <t>Stomach and Intestines V36Gy</t>
   </si>
   <si>
@@ -1192,6 +1189,42 @@
   </si>
   <si>
     <t>laterality</t>
+  </si>
+  <si>
+    <t>Proximal Trachea Maximum Dose</t>
+  </si>
+  <si>
+    <t>A54</t>
+  </si>
+  <si>
+    <t>Proximal Bronchial Tree Maximum Dose</t>
+  </si>
+  <si>
+    <t>B54</t>
+  </si>
+  <si>
+    <t>Proximal Trachea V15.6Gy</t>
+  </si>
+  <si>
+    <t>Proximal Bronchial Tree V15.6Gy</t>
+  </si>
+  <si>
+    <t>A45</t>
+  </si>
+  <si>
+    <t>B45</t>
+  </si>
+  <si>
+    <t>Proximal Trachea V60Gy</t>
+  </si>
+  <si>
+    <t>A46</t>
+  </si>
+  <si>
+    <t>Proximal Bronchial Tree V60Gy</t>
+  </si>
+  <si>
+    <t>B46</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1595,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1593,13 +1626,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s">
         <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>148</v>
@@ -1825,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,19 +2867,19 @@
         <v>142</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C44" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>292</v>
+      <c r="G44" s="12" t="s">
+        <v>313</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>101</v>
@@ -2857,22 +2890,22 @@
         <v>142</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="C45" t="s">
-        <v>178</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" t="s">
-        <v>275</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>293</v>
+        <v>314</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2880,22 +2913,22 @@
         <v>142</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>263</v>
+        <v>316</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" t="s">
-        <v>299</v>
-      </c>
-      <c r="G46" t="s">
-        <v>85</v>
+        <v>172</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>293</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2903,56 +2936,68 @@
         <v>142</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>264</v>
+        <v>317</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" t="s">
-        <v>276</v>
-      </c>
-      <c r="G47" t="s">
-        <v>87</v>
+        <v>168</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>293</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>121</v>
+      <c r="A48" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>220</v>
+        <v>263</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>121</v>
+        <v>299</v>
       </c>
       <c r="G48" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>121</v>
+      <c r="A49" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>221</v>
+        <v>264</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>276</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2960,53 +3005,84 @@
         <v>121</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F50" t="s">
         <v>121</v>
       </c>
       <c r="G50" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>141</v>
+      <c r="A51" t="s">
+        <v>121</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51"/>
+        <v>221</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" t="s">
+        <v>53</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>141</v>
+      <c r="A52" t="s">
+        <v>121</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C52"/>
+        <v>222</v>
+      </c>
+      <c r="F52" t="s">
+        <v>121</v>
+      </c>
+      <c r="G52" t="s">
+        <v>53</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C54"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C55"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C56"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3015,10 +3091,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,20 +3907,20 @@
       <c r="A36" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C36" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="7" t="s">
+      <c r="B36" t="s">
+        <v>312</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>284</v>
+      <c r="G36" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>101</v>
@@ -3855,22 +3931,22 @@
         <v>142</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="C37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" t="s">
-        <v>301</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>285</v>
+        <v>314</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3878,22 +3954,22 @@
         <v>142</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>263</v>
+        <v>320</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" t="s">
-        <v>299</v>
-      </c>
-      <c r="G38" t="s">
-        <v>286</v>
+        <v>172</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3901,56 +3977,68 @@
         <v>142</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" t="s">
-        <v>287</v>
+        <v>168</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>323</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>121</v>
+      <c r="A40" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>220</v>
+        <v>263</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>299</v>
       </c>
       <c r="G40" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>121</v>
+      <c r="A41" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>221</v>
+        <v>309</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>53</v>
+        <v>287</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3958,53 +4046,84 @@
         <v>121</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F42" t="s">
         <v>121</v>
       </c>
       <c r="G42" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>141</v>
+      <c r="A43" t="s">
+        <v>121</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43"/>
+        <v>221</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>141</v>
+      <c r="A44" t="s">
+        <v>121</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C44"/>
+        <v>222</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C45"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C46"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>